<commit_message>
Remove obsolete Excel file and update microplan compilation logic
- Deleted the temporary Excel file `ErectionCompiled_Output_testRun.xlsx` to clean up the project directory.
- Updated `microplan_compile.py` to remove unused parameters related to raw project writing, streamlining the function.
- Adjusted `pipeline_runner.py` to reflect the changes in the microplan compilation function.
- Added new Excel files for project reports and updated existing ones to ensure data accuracy and consistency.
</commit_message>
<xml_diff>
--- a/Test/Micro Plan - TA-416 Sep'25.xlsx
+++ b/Test/Micro Plan - TA-416 Sep'25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaushikb\Documents\Work\Git\Office-work-\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6342C0D-813C-487E-8089-A28BA47C7987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B48758C6-C2C1-4DAE-8171-1EEF5BAD5723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="757" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1610,69 +1610,69 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1688,6 +1688,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1695,9 +1698,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4780,41 +4780,41 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:33" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="187" t="s">
+      <c r="A18" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="187" t="s">
+      <c r="B18" s="172" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="183" t="s">
+      <c r="C18" s="169" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="187" t="s">
+      <c r="D18" s="172" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="183" t="s">
+      <c r="E18" s="169" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="183" t="s">
+      <c r="F18" s="169" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="187" t="s">
+      <c r="G18" s="172" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="174" t="s">
+      <c r="H18" s="184" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
-      <c r="K18" s="174"/>
-      <c r="L18" s="174"/>
-      <c r="M18" s="174"/>
-      <c r="N18" s="174"/>
-      <c r="O18" s="174"/>
+      <c r="I18" s="184"/>
+      <c r="J18" s="184"/>
+      <c r="K18" s="184"/>
+      <c r="L18" s="184"/>
+      <c r="M18" s="184"/>
+      <c r="N18" s="184"/>
+      <c r="O18" s="184"/>
       <c r="P18" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="R18" s="183" t="s">
+      <c r="R18" s="169" t="s">
         <v>36</v>
       </c>
       <c r="T18" s="178" t="s">
@@ -4838,33 +4838,33 @@
       </c>
     </row>
     <row r="19" spans="1:33" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="188"/>
-      <c r="B19" s="188"/>
-      <c r="C19" s="185"/>
-      <c r="D19" s="188"/>
-      <c r="E19" s="185"/>
-      <c r="F19" s="185"/>
-      <c r="G19" s="188"/>
-      <c r="H19" s="173" t="s">
+      <c r="A19" s="173"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="170"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="170"/>
+      <c r="F19" s="170"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="189" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="173"/>
-      <c r="J19" s="173" t="s">
+      <c r="I19" s="189"/>
+      <c r="J19" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="173"/>
-      <c r="L19" s="173" t="s">
+      <c r="K19" s="189"/>
+      <c r="L19" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="M19" s="173"/>
-      <c r="N19" s="171" t="s">
+      <c r="M19" s="189"/>
+      <c r="N19" s="185" t="s">
         <v>15</v>
       </c>
-      <c r="O19" s="171" t="s">
+      <c r="O19" s="185" t="s">
         <v>14</v>
       </c>
       <c r="P19" s="177"/>
-      <c r="R19" s="184"/>
+      <c r="R19" s="183"/>
       <c r="T19" s="175" t="s">
         <v>24</v>
       </c>
@@ -4904,13 +4904,13 @@
       <c r="AG19" s="182"/>
     </row>
     <row r="20" spans="1:33" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="189"/>
-      <c r="B20" s="188"/>
-      <c r="C20" s="185"/>
-      <c r="D20" s="188"/>
-      <c r="E20" s="186"/>
-      <c r="F20" s="186"/>
-      <c r="G20" s="188"/>
+      <c r="A20" s="174"/>
+      <c r="B20" s="173"/>
+      <c r="C20" s="170"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="171"/>
+      <c r="F20" s="171"/>
+      <c r="G20" s="173"/>
       <c r="H20" s="94" t="s">
         <v>10</v>
       </c>
@@ -4929,8 +4929,8 @@
       <c r="M20" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="N20" s="172"/>
-      <c r="O20" s="172"/>
+      <c r="N20" s="186"/>
+      <c r="O20" s="186"/>
       <c r="P20" s="44" t="s">
         <v>51</v>
       </c>
@@ -5218,7 +5218,7 @@
       <c r="D25" s="86"/>
       <c r="E25" s="102"/>
       <c r="F25" s="8"/>
-      <c r="G25" s="169"/>
+      <c r="G25" s="187"/>
       <c r="H25" s="100"/>
       <c r="I25" s="100"/>
       <c r="J25" s="100"/>
@@ -5276,7 +5276,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="103"/>
       <c r="F26" s="97"/>
-      <c r="G26" s="170"/>
+      <c r="G26" s="188"/>
       <c r="H26" s="100"/>
       <c r="I26" s="100"/>
       <c r="J26" s="100"/>
@@ -5631,13 +5631,16 @@
     <filterColumn colId="13" showButton="0"/>
   </autoFilter>
   <mergeCells count="29">
-    <mergeCell ref="F18:F20"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="H18:O18"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="U19:U20"/>
+    <mergeCell ref="V19:V20"/>
+    <mergeCell ref="W19:W20"/>
     <mergeCell ref="X19:X20"/>
     <mergeCell ref="P18:P19"/>
     <mergeCell ref="AA18:AF18"/>
@@ -5650,16 +5653,13 @@
     <mergeCell ref="R18:R19"/>
     <mergeCell ref="T18:Y18"/>
     <mergeCell ref="T19:T20"/>
-    <mergeCell ref="H18:O18"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="U19:U20"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="G25:G26"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B21">
@@ -6027,8 +6027,8 @@
   </sheetPr>
   <dimension ref="A1:AK38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:P1"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="88" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6154,7 +6154,10 @@
       <c r="O2" s="101">
         <v>861022</v>
       </c>
-      <c r="P2" s="101"/>
+      <c r="P2" s="101">
+        <f>O2*10%</f>
+        <v>86102.200000000012</v>
+      </c>
     </row>
     <row r="3" spans="1:37" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
@@ -6202,7 +6205,10 @@
       <c r="O3" s="101">
         <v>1610385.43</v>
       </c>
-      <c r="P3" s="101"/>
+      <c r="P3" s="101">
+        <f>O3*20%</f>
+        <v>322077.08600000001</v>
+      </c>
       <c r="Q3" s="149"/>
       <c r="R3" s="149"/>
       <c r="T3" s="150"/>
@@ -6386,7 +6392,10 @@
       <c r="O6" s="101">
         <v>712728.77</v>
       </c>
-      <c r="P6" s="101"/>
+      <c r="P6" s="101">
+        <f>O6*20%</f>
+        <v>142545.75400000002</v>
+      </c>
       <c r="Q6" s="142"/>
       <c r="R6" s="142"/>
       <c r="T6" s="155"/>
@@ -6634,7 +6643,10 @@
       <c r="O10" s="101">
         <v>974538</v>
       </c>
-      <c r="P10" s="101"/>
+      <c r="P10" s="101">
+        <f>O10*20%</f>
+        <v>194907.6</v>
+      </c>
       <c r="Q10" s="142"/>
       <c r="R10" s="142"/>
       <c r="T10" s="155"/>
@@ -7006,7 +7018,10 @@
       <c r="O16" s="101">
         <v>828626</v>
       </c>
-      <c r="P16" s="101"/>
+      <c r="P16" s="101">
+        <f>O16*20%</f>
+        <v>165725.20000000001</v>
+      </c>
       <c r="Q16" s="142"/>
       <c r="R16" s="142"/>
       <c r="T16" s="155"/>
@@ -7253,7 +7268,10 @@
       <c r="O20" s="101">
         <v>669569.35</v>
       </c>
-      <c r="P20" s="101"/>
+      <c r="P20" s="101">
+        <f>O20*20%</f>
+        <v>133913.87</v>
+      </c>
       <c r="Q20" s="142"/>
       <c r="R20" s="142"/>
       <c r="T20" s="155"/>
@@ -7437,7 +7455,10 @@
       <c r="O23" s="101">
         <v>837742</v>
       </c>
-      <c r="P23" s="101"/>
+      <c r="P23" s="101">
+        <f>O23*20%</f>
+        <v>167548.40000000002</v>
+      </c>
       <c r="Q23" s="142"/>
       <c r="R23" s="142"/>
       <c r="T23" s="155"/>
@@ -7748,7 +7769,10 @@
       <c r="O28" s="101">
         <v>450628</v>
       </c>
-      <c r="P28" s="101"/>
+      <c r="P28" s="101">
+        <f>O28*20%</f>
+        <v>90125.6</v>
+      </c>
       <c r="Q28" s="142"/>
       <c r="R28" s="142"/>
       <c r="T28" s="155"/>
@@ -9124,32 +9148,32 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:28" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="187" t="s">
+      <c r="A18" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="187" t="s">
+      <c r="B18" s="172" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="183" t="s">
+      <c r="C18" s="169" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="183" t="s">
+      <c r="D18" s="169" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="187" t="s">
+      <c r="E18" s="172" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="174" t="s">
+      <c r="F18" s="184" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="174"/>
-      <c r="H18" s="174"/>
-      <c r="I18" s="174"/>
-      <c r="J18" s="174"/>
+      <c r="G18" s="184"/>
+      <c r="H18" s="184"/>
+      <c r="I18" s="184"/>
+      <c r="J18" s="184"/>
       <c r="K18" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="M18" s="183" t="s">
+      <c r="M18" s="169" t="s">
         <v>36</v>
       </c>
       <c r="O18" s="178" t="s">
@@ -9173,24 +9197,24 @@
       </c>
     </row>
     <row r="19" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="188"/>
-      <c r="B19" s="188"/>
-      <c r="C19" s="185"/>
-      <c r="D19" s="188"/>
-      <c r="E19" s="188"/>
-      <c r="F19" s="195" t="s">
+      <c r="A19" s="173"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="170"/>
+      <c r="D19" s="173"/>
+      <c r="E19" s="173"/>
+      <c r="F19" s="196" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="196" t="s">
+      <c r="G19" s="197" t="s">
         <v>44</v>
       </c>
-      <c r="H19" s="197"/>
-      <c r="I19" s="196" t="s">
+      <c r="H19" s="198"/>
+      <c r="I19" s="197" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="197"/>
+      <c r="J19" s="198"/>
       <c r="K19" s="177"/>
-      <c r="M19" s="184"/>
+      <c r="M19" s="183"/>
       <c r="O19" s="175" t="s">
         <v>24</v>
       </c>
@@ -9230,12 +9254,12 @@
       <c r="AB19" s="182"/>
     </row>
     <row r="20" spans="1:28" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="188"/>
-      <c r="B20" s="188"/>
-      <c r="C20" s="185"/>
-      <c r="D20" s="188"/>
-      <c r="E20" s="188"/>
-      <c r="F20" s="195"/>
+      <c r="A20" s="173"/>
+      <c r="B20" s="173"/>
+      <c r="C20" s="170"/>
+      <c r="D20" s="173"/>
+      <c r="E20" s="173"/>
+      <c r="F20" s="196"/>
       <c r="G20" s="94" t="s">
         <v>10</v>
       </c>
@@ -9285,7 +9309,7 @@
       <c r="D21" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="198" t="s">
+      <c r="E21" s="195" t="s">
         <v>157</v>
       </c>
       <c r="F21" s="117">
@@ -9359,7 +9383,7 @@
       <c r="D22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="198"/>
+      <c r="E22" s="195"/>
       <c r="F22" s="117">
         <v>45913</v>
       </c>
@@ -9431,7 +9455,7 @@
       <c r="D23" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E23" s="198"/>
+      <c r="E23" s="195"/>
       <c r="F23" s="117">
         <v>45910</v>
       </c>
@@ -9503,7 +9527,7 @@
       <c r="D24" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E24" s="198"/>
+      <c r="E24" s="195"/>
       <c r="F24" s="117">
         <v>45927</v>
       </c>
@@ -9575,7 +9599,7 @@
       <c r="D25" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E25" s="198"/>
+      <c r="E25" s="195"/>
       <c r="F25" s="117">
         <v>45915</v>
       </c>
@@ -10270,18 +10294,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="W19:W20"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="O18:T18"/>
-    <mergeCell ref="V18:AA18"/>
-    <mergeCell ref="V19:V20"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="C18:C20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
     <mergeCell ref="AB18:AB19"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:H19"/>
@@ -10295,6 +10307,18 @@
     <mergeCell ref="Q19:Q20"/>
     <mergeCell ref="R19:R20"/>
     <mergeCell ref="S19:S20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="W19:W20"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="O18:T18"/>
+    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="V19:V20"/>
   </mergeCells>
   <conditionalFormatting sqref="C26:C27">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="4DT6">

</xml_diff>